<commit_message>
Made latest round of changes
</commit_message>
<xml_diff>
--- a/public/Publications.xlsx
+++ b/public/Publications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MJ/Development/dlj-clive-group-next/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4C1167-755F-5F43-AAE9-B965A3E0DEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61852A6E-AEDE-A347-B239-4EDCA1CA427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="661">
   <si>
     <t>Title</t>
   </si>
@@ -1759,9 +1759,6 @@
     <t>5125-5131</t>
   </si>
   <si>
-    <t>Reagent for Divalent Sulfur Protection: Preparation of 4-Methylbenzenesulfonothioic Acid, S-[[[(1,1-Dimethylethyl)dimethylsilyl]oxy]methyl] Ester</t>
-  </si>
-  <si>
     <t>Org. Synth.</t>
   </si>
   <si>
@@ -1988,6 +1985,25 @@
   </si>
   <si>
     <t>Conversion of 1,4-Diketones into &lt;i&gt;p&lt;/i&gt;-Disubstituted Benzenes</t>
+  </si>
+  <si>
+    <t>Reagent for Divalent Sulfur Protection: Preparation of 4-Methylbenzenesulfonothioic Acid, &lt;i&gt;S&lt;/i&gt;-[[[(1,1-Dimethylethyl)dimethylsilyl]oxy]methyl] Ester</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;90&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>10-24</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[See &lt;i&gt;J. Org. Chem.&lt;/i&gt; &lt;b&gt;1993&lt;/b&gt;, &lt;i&gt;58&lt;/i&gt;, 3472 for correction of typographical error.]
+</t>
+  </si>
+  <si>
+    <t>[See &lt;i&gt;J. Chem. Soc., Chem. Commun.&lt;/i&gt; &lt;b&gt;1993&lt;/b&gt;, 1240 for correction of typographical error.]</t>
   </si>
 </sst>
 </file>
@@ -2495,19 +2511,22 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2866,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G225"/>
+  <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A207" sqref="A207"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2884,30 +2903,33 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H1" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2926,11 +2948,11 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2947,7 +2969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2964,7 +2986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2981,7 +3003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -2998,7 +3020,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3015,7 +3037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -3032,7 +3054,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -3049,7 +3071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -3066,7 +3088,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3086,18 +3108,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D12" s="1">
         <v>1976</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -3114,7 +3136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -3134,7 +3156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -3151,7 +3173,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -3170,7 +3192,7 @@
     </row>
     <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>47</v>
@@ -3369,13 +3391,13 @@
     </row>
     <row r="28" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D28" s="1">
         <v>1980</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3480,13 +3502,13 @@
     </row>
     <row r="34" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D34" s="1">
         <v>1981</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -3639,7 +3661,7 @@
     </row>
     <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>100</v>
@@ -3824,7 +3846,7 @@
     </row>
     <row r="53" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>140</v>
@@ -3918,7 +3940,7 @@
     </row>
     <row r="58" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>155</v>
@@ -3955,7 +3977,7 @@
     </row>
     <row r="60" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>160</v>
@@ -4044,7 +4066,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>174</v>
       </c>
@@ -4064,7 +4086,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>178</v>
       </c>
@@ -4084,7 +4106,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>181</v>
       </c>
@@ -4104,7 +4126,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>184</v>
       </c>
@@ -4124,7 +4146,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -4141,7 +4163,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>190</v>
       </c>
@@ -4158,9 +4180,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>192</v>
@@ -4175,7 +4197,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>194</v>
       </c>
@@ -4195,7 +4217,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
@@ -4212,7 +4234,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>201</v>
       </c>
@@ -4232,7 +4254,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>203</v>
       </c>
@@ -4252,7 +4274,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>205</v>
       </c>
@@ -4272,7 +4294,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>207</v>
       </c>
@@ -4289,7 +4311,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>209</v>
       </c>
@@ -4308,8 +4330,11 @@
       <c r="F78" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="H78" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>212</v>
       </c>
@@ -4326,7 +4351,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>215</v>
       </c>
@@ -4343,7 +4368,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
@@ -4360,12 +4385,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>221</v>
       </c>
@@ -4382,7 +4407,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>224</v>
       </c>
@@ -4402,9 +4427,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>227</v>
@@ -4418,8 +4443,11 @@
       <c r="F85" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="H85" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>229</v>
       </c>
@@ -4439,7 +4467,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>232</v>
       </c>
@@ -4456,7 +4484,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>235</v>
       </c>
@@ -4473,7 +4501,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>238</v>
       </c>
@@ -4490,7 +4518,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>241</v>
       </c>
@@ -4510,7 +4538,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>244</v>
       </c>
@@ -4527,7 +4555,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>246</v>
       </c>
@@ -4547,9 +4575,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>249</v>
@@ -4567,7 +4595,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>221</v>
       </c>
@@ -4587,7 +4615,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>252</v>
       </c>
@@ -4607,7 +4635,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>256</v>
       </c>
@@ -4686,7 +4714,7 @@
     </row>
     <row r="100" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -4731,7 +4759,7 @@
     </row>
     <row r="103" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>274</v>
@@ -5738,7 +5766,7 @@
         <v>431</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D155" s="1">
         <v>2003</v>
@@ -6637,7 +6665,7 @@
     </row>
     <row r="201" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>566</v>
@@ -6737,35 +6765,35 @@
     </row>
     <row r="206" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>579</v>
+        <v>655</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>568</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D206" s="1">
         <v>2013</v>
       </c>
-      <c r="E206" s="1">
-        <v>90</v>
-      </c>
-      <c r="F206" s="3">
-        <v>45223</v>
+      <c r="E206" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="F206" s="5" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>582</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>284</v>
@@ -6777,15 +6805,15 @@
         <v>49</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>70</v>
@@ -6797,15 +6825,15 @@
         <v>78</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>588</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>527</v>
@@ -6817,15 +6845,15 @@
         <v>11</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>591</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>59</v>
@@ -6837,15 +6865,15 @@
         <v>69</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>594</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>70</v>
@@ -6857,15 +6885,15 @@
         <v>78</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>597</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>70</v>
@@ -6877,15 +6905,15 @@
         <v>80</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>600</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>70</v>
@@ -6897,15 +6925,15 @@
         <v>80</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>603</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>70</v>
@@ -6917,15 +6945,15 @@
         <v>80</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>606</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>119</v>
@@ -6937,15 +6965,15 @@
         <v>56</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>609</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>527</v>
@@ -6957,15 +6985,15 @@
         <v>17</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>612</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>70</v>
@@ -6977,15 +7005,15 @@
         <v>81</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>615</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>284</v>
@@ -6997,15 +7025,15 @@
         <v>52</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>618</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>70</v>
@@ -7017,15 +7045,15 @@
         <v>81</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>621</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>59</v>
@@ -7037,15 +7065,15 @@
         <v>74</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>624</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>119</v>
@@ -7057,15 +7085,15 @@
         <v>60</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>627</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>70</v>
@@ -7077,15 +7105,15 @@
         <v>84</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>630</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>70</v>
@@ -7097,15 +7125,15 @@
         <v>86</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>632</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>633</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>59</v>
@@ -7117,7 +7145,7 @@
         <v>133</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>